<commit_message>
add NL W8 data
</commit_message>
<xml_diff>
--- a/data/spss_files_nl.xlsx
+++ b/data/spss_files_nl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86936BC1-BF78-4B57-8607-764C352E9C23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0119AA0-E4B5-4C9F-9B86-D35916A3B173}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>country</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>20-090916_NL_Wave7_Final_v1_260321_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-090916_NL_Wave8_Final_v1_090421_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I16" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I17" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>nl_sr02_20200518_pA_wv02</v>
       </c>
       <c r="K3">
@@ -1082,6 +1085,36 @@
       <c r="I16" t="str">
         <f t="shared" si="0"/>
         <v>nl_sr15_20210331_pB_wv07</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>44295</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr16_20210409_pB_wv08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>